<commit_message>
add new meter abbreviations
new meter abbreviations M_AC_PF_COSPHI[1..x] and "M_AC_PF_TANPHI[1..x]" added
</commit_message>
<xml_diff>
--- a/import-specification/devices/meter.xlsx
+++ b/import-specification/devices/meter.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="136">
   <si>
     <t>Field Type</t>
   </si>
@@ -386,6 +386,45 @@
   </si>
   <si>
     <t>&lt;serial&gt;MET11.22.33&lt;/serial&gt;</t>
+  </si>
+  <si>
+    <t>M_AC_PF_COSPHI1</t>
+  </si>
+  <si>
+    <t>M_AC_PF_COSPHI2</t>
+  </si>
+  <si>
+    <t>M_AC_PF_COSPHI3</t>
+  </si>
+  <si>
+    <t>Power Factor 1 (cos(phi))</t>
+  </si>
+  <si>
+    <t>Power Factor 2 (cos(phi))</t>
+  </si>
+  <si>
+    <t>Power Factor 3 (cos(phi))</t>
+  </si>
+  <si>
+    <t>M_AC_PF_TANPHI1</t>
+  </si>
+  <si>
+    <t>M_AC_PF_TANPHI2</t>
+  </si>
+  <si>
+    <t>M_AC_PF_TANPHI3</t>
+  </si>
+  <si>
+    <t>Power Factor1 (tan(phi))</t>
+  </si>
+  <si>
+    <t>Power Factor2 (tan(phi))</t>
+  </si>
+  <si>
+    <t>Power Factor3 (tan(phi))</t>
+  </si>
+  <si>
+    <t>2.0.8</t>
   </si>
 </sst>
 </file>
@@ -544,9 +583,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -584,9 +623,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -621,7 +660,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -656,7 +695,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -830,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,13 +1416,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -1391,7 +1430,7 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -1399,13 +1438,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1413,7 +1452,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1421,13 +1460,13 @@
         <v>6</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1435,7 +1474,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1443,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1465,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1479,7 +1518,7 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1487,13 +1526,13 @@
         <v>6</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>84</v>
+        <v>133</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1501,7 +1540,7 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1509,13 +1548,13 @@
         <v>6</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1523,7 +1562,7 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1531,13 +1570,13 @@
         <v>6</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1553,13 +1592,13 @@
         <v>6</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1575,13 +1614,13 @@
         <v>6</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1597,13 +1636,13 @@
         <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -1619,13 +1658,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1641,13 +1680,13 @@
         <v>6</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -1663,13 +1702,13 @@
         <v>6</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -1685,13 +1724,13 @@
         <v>6</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
@@ -1707,13 +1746,13 @@
         <v>6</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1729,13 +1768,13 @@
         <v>6</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1751,13 +1790,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>95</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1773,13 +1812,13 @@
         <v>6</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1795,13 +1834,13 @@
         <v>6</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1817,13 +1856,13 @@
         <v>6</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1839,11 +1878,13 @@
         <v>6</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C45" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="D45" s="5" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1859,11 +1900,13 @@
         <v>6</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="D46" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1874,6 +1917,134 @@
         <v>118</v>
       </c>
     </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update meter, ppc import-specification
</commit_message>
<xml_diff>
--- a/import-specification/devices/meter.xlsx
+++ b/import-specification/devices/meter.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
   <si>
     <t>Field Type</t>
   </si>
@@ -341,13 +341,25 @@
     <t>M_EQ_CAP_INT_EXP</t>
   </si>
   <si>
-    <t>Reactive Energy Lead</t>
+    <t>Reactive energy exported capacitively per interval</t>
+  </si>
+  <si>
+    <t>M_EQ_CAP_INT_IMP</t>
+  </si>
+  <si>
+    <t>Reactive energy imported capacitively per interval</t>
   </si>
   <si>
     <t>M_EQ_IND_INT_EXP</t>
   </si>
   <si>
-    <t>Reactive Energy Lag</t>
+    <t>Reactive energy exported inductively per interval</t>
+  </si>
+  <si>
+    <t>M_EQ_IND_INT_IMP</t>
+  </si>
+  <si>
+    <t>Reactive energy imported inductively per interval</t>
   </si>
   <si>
     <t>STATE[1..x]</t>
@@ -719,7 +731,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1352,16 +1364,25 @@
       <c r="B41" t="s">
         <v>111</v>
       </c>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1369,9 +1390,6 @@
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1384,6 +1402,28 @@
       </c>
       <c r="D44" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>